<commit_message>
S01clean benchmarks almost done
</commit_message>
<xml_diff>
--- a/benchmarks/summary_seq.xlsx
+++ b/benchmarks/summary_seq.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -203,7 +203,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">In the benchmarks SQUARNA utilized the faster running config long.conf for the sequences longer than 500 nts, as the def.conf and alt.conf configs can take days to run on long sequences</t>
+      <t xml:space="preserve">In the benchmarks SQUARNA utilized the faster running config long.conf for the sequences longer than 1000 nts, as the def.conf and alt.conf configs can take days to run on long sequences</t>
     </r>
   </si>
   <si>
@@ -607,7 +607,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="J66" activeCellId="0" sqref="J66"/>
@@ -4103,15 +4103,15 @@
   </sheetPr>
   <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="14.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="13.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="11.52"/>

</xml_diff>

<commit_message>
updated Table S2, Table S3
</commit_message>
<xml_diff>
--- a/benchmarks/summary_seq.xlsx
+++ b/benchmarks/summary_seq.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="56">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -539,7 +539,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -602,8 +602,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
@@ -2597,20 +2597,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.31"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="11" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1019" min="11" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2627,34 +2627,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1" s="30" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J1" s="30" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="30" t="s">
         <v>13</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2673,7 +2667,7 @@
       </c>
       <c r="E2" s="32" t="n">
         <f aca="false">ROUND(2*E3*E4/(E3+E4),3)</f>
-        <v>0.777</v>
+        <v>0.704</v>
       </c>
       <c r="F2" s="32" t="n">
         <f aca="false">ROUND(2*F3*F4/(F3+F4),3)</f>
@@ -2681,7 +2675,7 @@
       </c>
       <c r="G2" s="32" t="n">
         <f aca="false">ROUND(2*G3*G4/(G3+G4),3)</f>
-        <v>0.704</v>
+        <v>0.711</v>
       </c>
       <c r="H2" s="32" t="n">
         <f aca="false">ROUND(2*H3*H4/(H3+H4),3)</f>
@@ -2689,7 +2683,7 @@
       </c>
       <c r="I2" s="32" t="n">
         <f aca="false">ROUND(2*I3*I4/(I3+I4),3)</f>
-        <v>0.793</v>
+        <v>0.777</v>
       </c>
       <c r="J2" s="33" t="n">
         <f aca="false">ROUND(2*J3*J4/(J3+J4),3)</f>
@@ -2697,19 +2691,11 @@
       </c>
       <c r="K2" s="32" t="n">
         <f aca="false">ROUND(2*K3*K4/(K3+K4),3)</f>
-        <v>0.711</v>
+        <v>0.793</v>
       </c>
       <c r="L2" s="32" t="n">
         <f aca="false">ROUND(2*L3*L4/(L3+L4),3)</f>
-        <v>0.709</v>
-      </c>
-      <c r="M2" s="32" t="n">
-        <f aca="false">ROUND(2*M3*M4/(M3+M4),3)</f>
         <v>0.789</v>
-      </c>
-      <c r="N2" s="32" t="n">
-        <f aca="false">ROUND(2*N3*N4/(N3+N4),3)</f>
-        <v>0.781</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,37 +2710,31 @@
         <v>0.721</v>
       </c>
       <c r="E3" s="26" t="n">
-        <v>0.774</v>
+        <v>0.697</v>
       </c>
       <c r="F3" s="26" t="n">
         <v>0.743</v>
       </c>
       <c r="G3" s="26" t="n">
-        <v>0.697</v>
+        <v>0.707</v>
       </c>
       <c r="H3" s="26" t="n">
         <v>0.771</v>
       </c>
       <c r="I3" s="26" t="n">
-        <v>0.795</v>
+        <v>0.774</v>
       </c>
       <c r="J3" s="34" t="n">
         <v>0.82</v>
       </c>
       <c r="K3" s="26" t="n">
-        <v>0.707</v>
+        <v>0.795</v>
       </c>
       <c r="L3" s="26" t="n">
-        <v>0.703</v>
-      </c>
-      <c r="M3" s="26" t="n">
         <v>0.772</v>
       </c>
-      <c r="N3" s="26" t="n">
-        <v>0.775</v>
-      </c>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8"/>
@@ -2768,34 +2748,28 @@
         <v>0.725</v>
       </c>
       <c r="E4" s="26" t="n">
-        <v>0.78</v>
+        <v>0.711</v>
       </c>
       <c r="F4" s="26" t="n">
         <v>0.742</v>
       </c>
       <c r="G4" s="26" t="n">
-        <v>0.711</v>
+        <v>0.716</v>
       </c>
       <c r="H4" s="26" t="n">
         <v>0.785</v>
       </c>
       <c r="I4" s="26" t="n">
-        <v>0.792</v>
+        <v>0.78</v>
       </c>
       <c r="J4" s="34" t="n">
         <v>0.819</v>
       </c>
       <c r="K4" s="26" t="n">
-        <v>0.716</v>
+        <v>0.792</v>
       </c>
       <c r="L4" s="26" t="n">
-        <v>0.715</v>
-      </c>
-      <c r="M4" s="26" t="n">
         <v>0.806</v>
-      </c>
-      <c r="N4" s="26" t="n">
-        <v>0.788</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2808,34 +2782,28 @@
         <v>0.5</v>
       </c>
       <c r="E5" s="26" t="n">
-        <v>0.5</v>
+        <v>37.6</v>
       </c>
       <c r="F5" s="26" t="n">
         <v>2.3</v>
       </c>
       <c r="G5" s="26" t="n">
-        <v>37.6</v>
+        <v>17</v>
       </c>
       <c r="H5" s="26" t="n">
         <v>36.7</v>
       </c>
       <c r="I5" s="26" t="n">
-        <v>26.5</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="26" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="26" t="n">
-        <v>17</v>
+        <v>26.5</v>
       </c>
       <c r="L5" s="26" t="n">
-        <v>10.4</v>
-      </c>
-      <c r="M5" s="26" t="n">
         <v>17.1</v>
-      </c>
-      <c r="N5" s="26" t="n">
-        <v>10.4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,7 +2822,7 @@
       </c>
       <c r="E6" s="32" t="n">
         <f aca="false">ROUND(2*E7*E8/(E7+E8),3)</f>
-        <v>0.776</v>
+        <v>0.723</v>
       </c>
       <c r="F6" s="32" t="n">
         <f aca="false">ROUND(2*F7*F8/(F7+F8),3)</f>
@@ -2862,35 +2830,27 @@
       </c>
       <c r="G6" s="32" t="n">
         <f aca="false">ROUND(2*G7*G8/(G7+G8),3)</f>
-        <v>0.723</v>
+        <v>0.691</v>
       </c>
       <c r="H6" s="32" t="n">
         <f aca="false">ROUND(2*H7*H8/(H7+H8),3)</f>
         <v>0.748</v>
       </c>
-      <c r="I6" s="33" t="n">
+      <c r="I6" s="32" t="n">
         <f aca="false">ROUND(2*I7*I8/(I7+I8),3)</f>
-        <v>0.789</v>
+        <v>0.776</v>
       </c>
       <c r="J6" s="32" t="n">
         <f aca="false">ROUND(2*J7*J8/(J7+J8),3)</f>
         <v>0.774</v>
       </c>
-      <c r="K6" s="32" t="n">
+      <c r="K6" s="33" t="n">
         <f aca="false">ROUND(2*K7*K8/(K7+K8),3)</f>
-        <v>0.691</v>
+        <v>0.789</v>
       </c>
       <c r="L6" s="32" t="n">
         <f aca="false">ROUND(2*L7*L8/(L7+L8),3)</f>
-        <v>0.665</v>
-      </c>
-      <c r="M6" s="32" t="n">
-        <f aca="false">ROUND(2*M7*M8/(M7+M8),3)</f>
         <v>0.771</v>
-      </c>
-      <c r="N6" s="32" t="n">
-        <f aca="false">ROUND(2*N7*N8/(N7+N8),3)</f>
-        <v>0.735</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,34 +2865,28 @@
         <v>0.694</v>
       </c>
       <c r="E7" s="26" t="n">
-        <v>0.735</v>
+        <v>0.697</v>
       </c>
       <c r="F7" s="26" t="n">
         <v>0.746</v>
       </c>
       <c r="G7" s="26" t="n">
-        <v>0.697</v>
+        <v>0.63</v>
       </c>
       <c r="H7" s="26" t="n">
         <v>0.722</v>
       </c>
-      <c r="I7" s="34" t="n">
-        <v>0.762</v>
+      <c r="I7" s="26" t="n">
+        <v>0.735</v>
       </c>
       <c r="J7" s="26" t="n">
         <v>0.734</v>
       </c>
-      <c r="K7" s="26" t="n">
-        <v>0.63</v>
+      <c r="K7" s="34" t="n">
+        <v>0.762</v>
       </c>
       <c r="L7" s="26" t="n">
-        <v>0.603</v>
-      </c>
-      <c r="M7" s="26" t="n">
         <v>0.705</v>
-      </c>
-      <c r="N7" s="26" t="n">
-        <v>0.672</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2947,34 +2901,28 @@
         <v>0.748</v>
       </c>
       <c r="E8" s="26" t="n">
-        <v>0.821</v>
+        <v>0.75</v>
       </c>
       <c r="F8" s="26" t="n">
         <v>0.757</v>
       </c>
       <c r="G8" s="26" t="n">
-        <v>0.75</v>
+        <v>0.766</v>
       </c>
       <c r="H8" s="26" t="n">
         <v>0.775</v>
       </c>
       <c r="I8" s="26" t="n">
-        <v>0.819</v>
+        <v>0.821</v>
       </c>
       <c r="J8" s="26" t="n">
         <v>0.818</v>
       </c>
       <c r="K8" s="26" t="n">
-        <v>0.766</v>
-      </c>
-      <c r="L8" s="26" t="n">
-        <v>0.742</v>
-      </c>
-      <c r="M8" s="34" t="n">
+        <v>0.819</v>
+      </c>
+      <c r="L8" s="34" t="n">
         <v>0.851</v>
-      </c>
-      <c r="N8" s="26" t="n">
-        <v>0.812</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2986,35 +2934,29 @@
       <c r="D9" s="26" t="n">
         <v>6.2</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>29</v>
+      <c r="E9" s="23" t="n">
+        <v>4452.3</v>
       </c>
       <c r="F9" s="26" t="n">
         <v>8394.6</v>
       </c>
-      <c r="G9" s="23" t="n">
-        <v>4452.3</v>
+      <c r="G9" s="26" t="s">
+        <v>31</v>
       </c>
       <c r="H9" s="26" t="n">
         <v>4600.9</v>
       </c>
-      <c r="I9" s="26" t="n">
-        <v>267.3</v>
+      <c r="I9" s="26" t="s">
+        <v>29</v>
       </c>
       <c r="J9" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="26" t="s">
-        <v>31</v>
+      <c r="K9" s="26" t="n">
+        <v>267.3</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="26" t="s">
         <v>34</v>
-      </c>
-      <c r="N9" s="26" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3030,6 +2972,7 @@
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
@@ -3044,6 +2987,7 @@
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27"/>
@@ -3056,6 +3000,7 @@
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="28" t="s">
@@ -3070,6 +3015,7 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27"/>
@@ -3082,6 +3028,7 @@
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27"/>
@@ -3094,6 +3041,7 @@
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="27"/>
@@ -3106,6 +3054,7 @@
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28"/>
@@ -3118,6 +3067,7 @@
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
       <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3125,12 +3075,12 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="A11:J12"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A15:J16"/>
-    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A11:K12"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="A15:K16"/>
+    <mergeCell ref="A17:K17"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3147,10 +3097,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:L33"/>
+  <dimension ref="A2:J29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O25" activeCellId="0" sqref="O25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3162,9 +3112,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="12.78"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="15.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="11" style="6" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3180,8 +3128,6 @@
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
@@ -3191,34 +3137,28 @@
         <v>3</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>6</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="30" t="s">
         <v>13</v>
-      </c>
-      <c r="L3" s="30" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3229,110 +3169,92 @@
         <v>1</v>
       </c>
       <c r="C4" s="37" t="n">
-        <v>0.714748633931574</v>
+        <v>0.958</v>
       </c>
       <c r="D4" s="37" t="n">
-        <v>0.957540649097073</v>
+        <v>0.715</v>
       </c>
       <c r="E4" s="37" t="n">
-        <v>0.474379809304658</v>
+        <v>0.474</v>
       </c>
       <c r="F4" s="37" t="n">
-        <v>0.818422944570017</v>
+        <v>0.295</v>
       </c>
       <c r="G4" s="38" t="n">
-        <v>0.00443030753633748</v>
-      </c>
-      <c r="H4" s="37" t="n">
-        <v>0.295432540095121</v>
+        <v>0.00443</v>
+      </c>
+      <c r="H4" s="38" t="n">
+        <v>0.00428</v>
       </c>
       <c r="I4" s="38" t="n">
-        <v>0.00323966900068798</v>
+        <v>0.00324</v>
       </c>
       <c r="J4" s="38" t="n">
-        <v>0.00427870901149946</v>
-      </c>
-      <c r="K4" s="38" t="n">
-        <v>4.75094168310171E-006</v>
-      </c>
-      <c r="L4" s="38" t="n">
-        <v>0.00723381490170699</v>
+        <v>4.75E-006</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="37" t="n">
-        <v>0.714748633931574</v>
+        <v>0.958</v>
       </c>
       <c r="C5" s="37" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="37" t="n">
-        <v>0.75389196237731</v>
+        <v>0.754</v>
       </c>
       <c r="E5" s="37" t="n">
-        <v>0.706002363672323</v>
+        <v>0.504</v>
       </c>
       <c r="F5" s="37" t="n">
-        <v>0.533444263236488</v>
+        <v>0.315</v>
       </c>
       <c r="G5" s="38" t="n">
-        <v>0.00717013892723614</v>
-      </c>
-      <c r="H5" s="37" t="n">
-        <v>0.456018656321116</v>
+        <v>0.00467</v>
+      </c>
+      <c r="H5" s="38" t="n">
+        <v>0.00449</v>
       </c>
       <c r="I5" s="38" t="n">
-        <v>0.00510172041114741</v>
+        <v>0.00339</v>
       </c>
       <c r="J5" s="38" t="n">
-        <v>0.00684192709300344</v>
-      </c>
-      <c r="K5" s="38" t="n">
-        <v>3.6884780117404E-006</v>
-      </c>
-      <c r="L5" s="37" t="n">
-        <v>0.0117679295708231</v>
+        <v>4.34E-006</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="37" t="n">
-        <v>0.957540649097073</v>
+        <v>0.715</v>
       </c>
       <c r="C6" s="37" t="n">
-        <v>0.75389196237731</v>
+        <v>0.754</v>
       </c>
       <c r="D6" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="37" t="n">
-        <v>0.504043652412933</v>
+        <v>0.706</v>
       </c>
       <c r="F6" s="37" t="n">
-        <v>0.77401540075107</v>
+        <v>0.456</v>
       </c>
       <c r="G6" s="38" t="n">
-        <v>0.00466833332930197</v>
-      </c>
-      <c r="H6" s="37" t="n">
-        <v>0.314996170649219</v>
+        <v>0.00717</v>
+      </c>
+      <c r="H6" s="38" t="n">
+        <v>0.00684</v>
       </c>
       <c r="I6" s="38" t="n">
-        <v>0.00338816682933919</v>
+        <v>0.0051</v>
       </c>
       <c r="J6" s="38" t="n">
-        <v>0.00449186238377379</v>
-      </c>
-      <c r="K6" s="38" t="n">
-        <v>4.33721427403821E-006</v>
-      </c>
-      <c r="L6" s="38" t="n">
-        <v>0.00762531805688691</v>
+        <v>3.69E-006</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3340,75 +3262,63 @@
         <v>10</v>
       </c>
       <c r="B7" s="37" t="n">
-        <v>0.474379809304658</v>
+        <v>0.474</v>
       </c>
       <c r="C7" s="37" t="n">
-        <v>0.706002363672323</v>
+        <v>0.504</v>
       </c>
       <c r="D7" s="37" t="n">
-        <v>0.504043652412933</v>
+        <v>0.706</v>
       </c>
       <c r="E7" s="37" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="37" t="n">
-        <v>0.324997766881125</v>
+        <v>0.7</v>
       </c>
       <c r="G7" s="37" t="n">
-        <v>0.019630195718658</v>
+        <v>0.0196</v>
       </c>
       <c r="H7" s="37" t="n">
-        <v>0.69974052235936</v>
+        <v>0.0197</v>
       </c>
       <c r="I7" s="37" t="n">
-        <v>0.0152803420223846</v>
-      </c>
-      <c r="J7" s="37" t="n">
-        <v>0.0197189593076012</v>
-      </c>
-      <c r="K7" s="38" t="n">
-        <v>2.23811693965422E-005</v>
-      </c>
-      <c r="L7" s="37" t="n">
-        <v>0.032662507025007</v>
+        <v>0.0153</v>
+      </c>
+      <c r="J7" s="38" t="n">
+        <v>2.24E-005</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" s="37" t="n">
-        <v>0.818422944570017</v>
+        <v>0.295</v>
       </c>
       <c r="C8" s="37" t="n">
-        <v>0.533444263236488</v>
+        <v>0.315</v>
       </c>
       <c r="D8" s="37" t="n">
-        <v>0.77401540075107</v>
+        <v>0.456</v>
       </c>
       <c r="E8" s="37" t="n">
-        <v>0.324997766881125</v>
+        <v>0.7</v>
       </c>
       <c r="F8" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="38" t="n">
-        <v>0.00152510157074715</v>
+      <c r="G8" s="37" t="n">
+        <v>0.0627</v>
       </c>
       <c r="H8" s="37" t="n">
-        <v>0.18901939844168</v>
-      </c>
-      <c r="I8" s="38" t="n">
-        <v>0.000992284984305612</v>
+        <v>0.0669</v>
+      </c>
+      <c r="I8" s="37" t="n">
+        <v>0.0551</v>
       </c>
       <c r="J8" s="38" t="n">
-        <v>0.00137542191799129</v>
-      </c>
-      <c r="K8" s="38" t="n">
-        <v>5.20499761659124E-007</v>
-      </c>
-      <c r="L8" s="38" t="n">
-        <v>0.00242605619002221</v>
+        <v>0.000339</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,75 +3326,63 @@
         <v>4</v>
       </c>
       <c r="B9" s="38" t="n">
-        <v>0.00443030753633748</v>
+        <v>0.00443</v>
       </c>
       <c r="C9" s="38" t="n">
-        <v>0.00717013892723614</v>
+        <v>0.00467</v>
       </c>
       <c r="D9" s="38" t="n">
-        <v>0.00466833332930197</v>
+        <v>0.00717</v>
       </c>
       <c r="E9" s="37" t="n">
-        <v>0.019630195718658</v>
-      </c>
-      <c r="F9" s="38" t="n">
-        <v>0.00152510157074715</v>
+        <v>0.0196</v>
+      </c>
+      <c r="F9" s="37" t="n">
+        <v>0.0627</v>
       </c>
       <c r="G9" s="37" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="37" t="n">
-        <v>0.0627099810406153</v>
+        <v>0.903</v>
       </c>
       <c r="I9" s="37" t="n">
-        <v>0.961150881676787</v>
+        <v>0.961</v>
       </c>
       <c r="J9" s="37" t="n">
-        <v>0.903306505371742</v>
-      </c>
-      <c r="K9" s="37" t="n">
-        <v>0.130863427296855</v>
-      </c>
-      <c r="L9" s="37" t="n">
-        <v>0.70964724507124</v>
+        <v>0.131</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="37" t="n">
-        <v>0.295432540095121</v>
-      </c>
-      <c r="C10" s="37" t="n">
-        <v>0.456018656321116</v>
-      </c>
-      <c r="D10" s="37" t="n">
-        <v>0.314996170649219</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="38" t="n">
+        <v>0.00428</v>
+      </c>
+      <c r="C10" s="38" t="n">
+        <v>0.00449</v>
+      </c>
+      <c r="D10" s="38" t="n">
+        <v>0.00684</v>
       </c>
       <c r="E10" s="37" t="n">
-        <v>0.69974052235936</v>
+        <v>0.0197</v>
       </c>
       <c r="F10" s="37" t="n">
-        <v>0.18901939844168</v>
+        <v>0.0669</v>
       </c>
       <c r="G10" s="37" t="n">
-        <v>0.0627099810406153</v>
+        <v>0.903</v>
       </c>
       <c r="H10" s="37" t="n">
         <v>1</v>
       </c>
       <c r="I10" s="37" t="n">
-        <v>0.0551399230478992</v>
+        <v>0.938</v>
       </c>
       <c r="J10" s="37" t="n">
-        <v>0.0668864978432009</v>
-      </c>
-      <c r="K10" s="38" t="n">
-        <v>0.000338676746418268</v>
-      </c>
-      <c r="L10" s="37" t="n">
-        <v>0.102562435042994</v>
+        <v>0.078</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3492,635 +3390,409 @@
         <v>8</v>
       </c>
       <c r="B11" s="38" t="n">
-        <v>0.00323966900068798</v>
+        <v>0.00324</v>
       </c>
       <c r="C11" s="38" t="n">
-        <v>0.00510172041114741</v>
+        <v>0.00339</v>
       </c>
       <c r="D11" s="38" t="n">
-        <v>0.00338816682933919</v>
+        <v>0.0051</v>
       </c>
       <c r="E11" s="37" t="n">
-        <v>0.0152803420223846</v>
-      </c>
-      <c r="F11" s="38" t="n">
-        <v>0.000992284984305612</v>
+        <v>0.0153</v>
+      </c>
+      <c r="F11" s="37" t="n">
+        <v>0.0551</v>
       </c>
       <c r="G11" s="37" t="n">
-        <v>0.961150881676787</v>
+        <v>0.961</v>
       </c>
       <c r="H11" s="37" t="n">
-        <v>0.0551399230478992</v>
+        <v>0.938</v>
       </c>
       <c r="I11" s="37" t="n">
         <v>1</v>
       </c>
       <c r="J11" s="37" t="n">
-        <v>0.937785636744972</v>
-      </c>
-      <c r="K11" s="37" t="n">
-        <v>0.0898785408595605</v>
-      </c>
-      <c r="L11" s="37" t="n">
-        <v>0.729712574749583</v>
+        <v>0.0899</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="30" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B12" s="38" t="n">
-        <v>0.00427870901149946</v>
+        <v>4.75E-006</v>
       </c>
       <c r="C12" s="38" t="n">
-        <v>0.00684192709300344</v>
+        <v>4.34E-006</v>
       </c>
       <c r="D12" s="38" t="n">
-        <v>0.00449186238377379</v>
-      </c>
-      <c r="E12" s="37" t="n">
-        <v>0.0197189593076012</v>
+        <v>3.69E-006</v>
+      </c>
+      <c r="E12" s="38" t="n">
+        <v>2.24E-005</v>
       </c>
       <c r="F12" s="38" t="n">
-        <v>0.00137542191799129</v>
+        <v>0.000339</v>
       </c>
       <c r="G12" s="37" t="n">
-        <v>0.903306505371742</v>
+        <v>0.131</v>
       </c>
       <c r="H12" s="37" t="n">
-        <v>0.0668864978432009</v>
+        <v>0.078</v>
       </c>
       <c r="I12" s="37" t="n">
-        <v>0.937785636744972</v>
+        <v>0.0899</v>
       </c>
       <c r="J12" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="K12" s="37" t="n">
-        <v>0.0779524618889699</v>
-      </c>
-      <c r="L12" s="37" t="n">
-        <v>0.792682079644613</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="38" t="n">
-        <v>4.75094168310171E-006</v>
-      </c>
-      <c r="C13" s="38" t="n">
-        <v>3.6884780117404E-006</v>
-      </c>
-      <c r="D13" s="38" t="n">
-        <v>4.33721427403821E-006</v>
-      </c>
-      <c r="E13" s="38" t="n">
-        <v>2.23811693965422E-005</v>
-      </c>
-      <c r="F13" s="38" t="n">
-        <v>5.20499761659124E-007</v>
-      </c>
-      <c r="G13" s="37" t="n">
-        <v>0.130863427296855</v>
-      </c>
-      <c r="H13" s="38" t="n">
-        <v>0.000338676746418268</v>
-      </c>
-      <c r="I13" s="37" t="n">
-        <v>0.0898785408595605</v>
-      </c>
-      <c r="J13" s="37" t="n">
-        <v>0.0779524618889699</v>
-      </c>
-      <c r="K13" s="37" t="n">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="37" t="n">
-        <v>0.0342482084527107</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="38" t="n">
-        <v>0.00723381490170699</v>
-      </c>
-      <c r="C14" s="37" t="n">
-        <v>0.0117679295708231</v>
-      </c>
-      <c r="D14" s="38" t="n">
-        <v>0.00762531805688691</v>
-      </c>
-      <c r="E14" s="37" t="n">
-        <v>0.032662507025007</v>
-      </c>
-      <c r="F14" s="38" t="n">
-        <v>0.00242605619002221</v>
-      </c>
-      <c r="G14" s="37" t="n">
-        <v>0.70964724507124</v>
-      </c>
-      <c r="H14" s="37" t="n">
-        <v>0.102562435042994</v>
-      </c>
-      <c r="I14" s="37" t="n">
-        <v>0.729712574749583</v>
-      </c>
-      <c r="J14" s="37" t="n">
-        <v>0.792682079644613</v>
-      </c>
-      <c r="K14" s="37" t="n">
-        <v>0.0342482084527107</v>
-      </c>
-      <c r="L14" s="37" t="n">
+      <c r="C16" s="37" t="n">
+        <v>0.782</v>
+      </c>
+      <c r="D16" s="37" t="n">
+        <v>0.711</v>
+      </c>
+      <c r="E16" s="37" t="n">
+        <v>0.861</v>
+      </c>
+      <c r="F16" s="37" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="G16" s="37" t="n">
+        <v>0.247</v>
+      </c>
+      <c r="H16" s="37" t="n">
+        <v>0.0247</v>
+      </c>
+      <c r="I16" s="37" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="J16" s="37" t="n">
+        <v>0.0639</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="37" t="n">
+        <v>0.782</v>
+      </c>
+      <c r="C17" s="37" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="L17" s="30" t="s">
-        <v>14</v>
+      <c r="D17" s="37" t="n">
+        <v>0.496</v>
+      </c>
+      <c r="E17" s="37" t="n">
+        <v>0.919</v>
+      </c>
+      <c r="F17" s="37" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="37" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="H17" s="38" t="n">
+        <v>0.00858</v>
+      </c>
+      <c r="I17" s="37" t="n">
+        <v>0.0653</v>
+      </c>
+      <c r="J17" s="37" t="n">
+        <v>0.0272</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="30" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B18" s="37" t="n">
+        <v>0.711</v>
+      </c>
+      <c r="C18" s="37" t="n">
+        <v>0.496</v>
+      </c>
+      <c r="D18" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C18" s="37" t="n">
-        <v>0.711411801097545</v>
-      </c>
-      <c r="D18" s="37" t="n">
-        <v>0.782479648590841</v>
-      </c>
       <c r="E18" s="37" t="n">
-        <v>0.860527532024685</v>
+        <v>0.569</v>
       </c>
       <c r="F18" s="37" t="n">
-        <v>0.845679510188673</v>
+        <v>0.287</v>
       </c>
       <c r="G18" s="37" t="n">
-        <v>0.247102821207723</v>
+        <v>0.372</v>
       </c>
       <c r="H18" s="37" t="n">
-        <v>0.188678920519769</v>
+        <v>0.0321</v>
       </c>
       <c r="I18" s="37" t="n">
-        <v>0.133534414972666</v>
+        <v>0.203</v>
       </c>
       <c r="J18" s="37" t="n">
-        <v>0.0247248784644662</v>
-      </c>
-      <c r="K18" s="37" t="n">
-        <v>0.0638594258001617</v>
-      </c>
-      <c r="L18" s="37" t="n">
-        <v>0.162148452369083</v>
+        <v>0.0933</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="30" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B19" s="37" t="n">
-        <v>0.711411801097545</v>
+        <v>0.861</v>
       </c>
       <c r="C19" s="37" t="n">
+        <v>0.919</v>
+      </c>
+      <c r="D19" s="37" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="E19" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="37" t="n">
-        <v>0.49589998730605</v>
-      </c>
-      <c r="E19" s="37" t="n">
-        <v>0.569165401380672</v>
-      </c>
       <c r="F19" s="37" t="n">
-        <v>0.558715005951011</v>
+        <v>0.126</v>
       </c>
       <c r="G19" s="37" t="n">
-        <v>0.372193112464921</v>
+        <v>0.173</v>
       </c>
       <c r="H19" s="37" t="n">
-        <v>0.287320483839445</v>
+        <v>0.0124</v>
       </c>
       <c r="I19" s="37" t="n">
-        <v>0.203031022405904</v>
+        <v>0.0845</v>
       </c>
       <c r="J19" s="37" t="n">
-        <v>0.0320950448749731</v>
-      </c>
-      <c r="K19" s="37" t="n">
-        <v>0.0933498184951495</v>
-      </c>
-      <c r="L19" s="37" t="n">
-        <v>0.247330919728258</v>
+        <v>0.0369</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20" s="37" t="n">
-        <v>0.782479648590841</v>
+        <v>0.189</v>
       </c>
       <c r="C20" s="37" t="n">
-        <v>0.49589998730605</v>
+        <v>0.1</v>
       </c>
       <c r="D20" s="37" t="n">
+        <v>0.287</v>
+      </c>
+      <c r="E20" s="37" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="F20" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="37" t="n">
-        <v>0.919278145720976</v>
-      </c>
-      <c r="F20" s="37" t="n">
-        <v>0.93696127120142</v>
-      </c>
       <c r="G20" s="37" t="n">
-        <v>0.140986001067181</v>
+        <v>0.899</v>
       </c>
       <c r="H20" s="37" t="n">
-        <v>0.100143373663272</v>
+        <v>0.334</v>
       </c>
       <c r="I20" s="37" t="n">
-        <v>0.065305830080741</v>
-      </c>
-      <c r="J20" s="38" t="n">
-        <v>0.00858490908541508</v>
-      </c>
-      <c r="K20" s="37" t="n">
-        <v>0.027245153436443</v>
-      </c>
-      <c r="L20" s="37" t="n">
-        <v>0.0827129880713282</v>
+        <v>0.862</v>
+      </c>
+      <c r="J20" s="37" t="n">
+        <v>0.573</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="30" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B21" s="37" t="n">
-        <v>0.860527532024685</v>
+        <v>0.247</v>
       </c>
       <c r="C21" s="37" t="n">
-        <v>0.569165401380672</v>
+        <v>0.141</v>
       </c>
       <c r="D21" s="37" t="n">
-        <v>0.919278145720976</v>
+        <v>0.372</v>
       </c>
       <c r="E21" s="37" t="n">
+        <v>0.173</v>
+      </c>
+      <c r="F21" s="37" t="n">
+        <v>0.899</v>
+      </c>
+      <c r="G21" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="37" t="n">
-        <v>0.983176080002237</v>
-      </c>
-      <c r="G21" s="37" t="n">
-        <v>0.173172428425893</v>
-      </c>
       <c r="H21" s="37" t="n">
-        <v>0.126110813420478</v>
+        <v>0.294</v>
       </c>
       <c r="I21" s="37" t="n">
-        <v>0.0845423446402642</v>
+        <v>0.767</v>
       </c>
       <c r="J21" s="37" t="n">
-        <v>0.0124154571363616</v>
-      </c>
-      <c r="K21" s="37" t="n">
-        <v>0.0368705770232143</v>
-      </c>
-      <c r="L21" s="37" t="n">
-        <v>0.105581018219611</v>
+        <v>0.504</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22" s="37" t="n">
-        <v>0.845679510188673</v>
-      </c>
-      <c r="C22" s="37" t="n">
-        <v>0.558715005951011</v>
+        <v>0.0247</v>
+      </c>
+      <c r="C22" s="38" t="n">
+        <v>0.00858</v>
       </c>
       <c r="D22" s="37" t="n">
-        <v>0.93696127120142</v>
+        <v>0.0321</v>
       </c>
       <c r="E22" s="37" t="n">
-        <v>0.983176080002237</v>
+        <v>0.0124</v>
       </c>
       <c r="F22" s="37" t="n">
+        <v>0.334</v>
+      </c>
+      <c r="G22" s="37" t="n">
+        <v>0.294</v>
+      </c>
+      <c r="H22" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="G22" s="37" t="n">
-        <v>0.171497569852203</v>
-      </c>
-      <c r="H22" s="37" t="n">
-        <v>0.125466720983247</v>
-      </c>
       <c r="I22" s="37" t="n">
-        <v>0.0846724292622886</v>
+        <v>0.415</v>
       </c>
       <c r="J22" s="37" t="n">
-        <v>0.0129661661798297</v>
-      </c>
-      <c r="K22" s="37" t="n">
-        <v>0.0374668281879344</v>
-      </c>
-      <c r="L22" s="37" t="n">
-        <v>0.105357105314806</v>
+        <v>0.696</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B23" s="37" t="n">
-        <v>0.247102821207723</v>
+        <v>0.134</v>
       </c>
       <c r="C23" s="37" t="n">
-        <v>0.372193112464921</v>
+        <v>0.0653</v>
       </c>
       <c r="D23" s="37" t="n">
-        <v>0.140986001067181</v>
+        <v>0.203</v>
       </c>
       <c r="E23" s="37" t="n">
-        <v>0.173172428425893</v>
+        <v>0.0845</v>
       </c>
       <c r="F23" s="37" t="n">
-        <v>0.171497569852203</v>
+        <v>0.862</v>
       </c>
       <c r="G23" s="37" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="H23" s="37" t="n">
+        <v>0.415</v>
+      </c>
+      <c r="I23" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="H23" s="37" t="n">
-        <v>0.899228063480899</v>
-      </c>
-      <c r="I23" s="37" t="n">
-        <v>0.767043279737067</v>
-      </c>
       <c r="J23" s="37" t="n">
-        <v>0.293768338770775</v>
-      </c>
-      <c r="K23" s="37" t="n">
-        <v>0.503816606491465</v>
-      </c>
-      <c r="L23" s="37" t="n">
-        <v>0.84428477092991</v>
+        <v>0.687</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="30" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B24" s="37" t="n">
-        <v>0.188678920519769</v>
+        <v>0.0639</v>
       </c>
       <c r="C24" s="37" t="n">
-        <v>0.287320483839445</v>
+        <v>0.0272</v>
       </c>
       <c r="D24" s="37" t="n">
-        <v>0.100143373663272</v>
+        <v>0.0933</v>
       </c>
       <c r="E24" s="37" t="n">
-        <v>0.126110813420478</v>
+        <v>0.0369</v>
       </c>
       <c r="F24" s="37" t="n">
-        <v>0.125466720983247</v>
+        <v>0.573</v>
       </c>
       <c r="G24" s="37" t="n">
-        <v>0.899228063480899</v>
+        <v>0.504</v>
       </c>
       <c r="H24" s="37" t="n">
+        <v>0.696</v>
+      </c>
+      <c r="I24" s="37" t="n">
+        <v>0.687</v>
+      </c>
+      <c r="J24" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="37" t="n">
-        <v>0.861951470829309</v>
-      </c>
-      <c r="J24" s="37" t="n">
-        <v>0.334283129136246</v>
-      </c>
-      <c r="K24" s="37" t="n">
-        <v>0.572556107403261</v>
-      </c>
-      <c r="L24" s="37" t="n">
-        <v>0.943790118641581</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="37" t="n">
-        <v>0.133534414972666</v>
-      </c>
-      <c r="C25" s="37" t="n">
-        <v>0.203031022405904</v>
-      </c>
-      <c r="D25" s="37" t="n">
-        <v>0.065305830080741</v>
-      </c>
-      <c r="E25" s="37" t="n">
-        <v>0.0845423446402642</v>
-      </c>
-      <c r="F25" s="37" t="n">
-        <v>0.0846724292622886</v>
-      </c>
-      <c r="G25" s="37" t="n">
-        <v>0.767043279737067</v>
-      </c>
-      <c r="H25" s="37" t="n">
-        <v>0.861951470829309</v>
-      </c>
-      <c r="I25" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="J25" s="37" t="n">
-        <v>0.415095566094501</v>
-      </c>
-      <c r="K25" s="37" t="n">
-        <v>0.686609758608552</v>
-      </c>
-      <c r="L25" s="37" t="n">
-        <v>0.916405547310892</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="37" t="n">
-        <v>0.0247248784644662</v>
-      </c>
-      <c r="C26" s="37" t="n">
-        <v>0.0320950448749731</v>
-      </c>
-      <c r="D26" s="38" t="n">
-        <v>0.00858490908541508</v>
-      </c>
-      <c r="E26" s="37" t="n">
-        <v>0.0124154571363616</v>
-      </c>
-      <c r="F26" s="37" t="n">
-        <v>0.0129661661798297</v>
-      </c>
-      <c r="G26" s="37" t="n">
-        <v>0.293768338770775</v>
-      </c>
-      <c r="H26" s="37" t="n">
-        <v>0.334283129136246</v>
-      </c>
-      <c r="I26" s="37" t="n">
-        <v>0.415095566094501</v>
-      </c>
-      <c r="J26" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="K26" s="37" t="n">
-        <v>0.695659319592635</v>
-      </c>
-      <c r="L26" s="37" t="n">
-        <v>0.360227836965591</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="37" t="n">
-        <v>0.0638594258001617</v>
-      </c>
-      <c r="C27" s="37" t="n">
-        <v>0.0933498184951495</v>
-      </c>
-      <c r="D27" s="37" t="n">
-        <v>0.027245153436443</v>
-      </c>
-      <c r="E27" s="37" t="n">
-        <v>0.0368705770232143</v>
-      </c>
-      <c r="F27" s="37" t="n">
-        <v>0.0374668281879344</v>
-      </c>
-      <c r="G27" s="37" t="n">
-        <v>0.503816606491465</v>
-      </c>
-      <c r="H27" s="37" t="n">
-        <v>0.572556107403261</v>
-      </c>
-      <c r="I27" s="37" t="n">
-        <v>0.686609758608552</v>
-      </c>
-      <c r="J27" s="37" t="n">
-        <v>0.695659319592635</v>
-      </c>
-      <c r="K27" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="L27" s="37" t="n">
-        <v>0.61404212613652</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="37" t="n">
-        <v>0.162148452369083</v>
-      </c>
-      <c r="C28" s="37" t="n">
-        <v>0.247330919728258</v>
-      </c>
-      <c r="D28" s="37" t="n">
-        <v>0.0827129880713282</v>
-      </c>
-      <c r="E28" s="37" t="n">
-        <v>0.105581018219611</v>
-      </c>
-      <c r="F28" s="37" t="n">
-        <v>0.105357105314806</v>
-      </c>
-      <c r="G28" s="37" t="n">
-        <v>0.84428477092991</v>
-      </c>
-      <c r="H28" s="37" t="n">
-        <v>0.943790118641581</v>
-      </c>
-      <c r="I28" s="37" t="n">
-        <v>0.916405547310892</v>
-      </c>
-      <c r="J28" s="37" t="n">
-        <v>0.360227836965591</v>
-      </c>
-      <c r="K28" s="37" t="n">
-        <v>0.61404212613652</v>
-      </c>
-      <c r="L28" s="37" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A14:J14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>